<commit_message>
Fix disorder parameter implementation
</commit_message>
<xml_diff>
--- a/src/site/mining.xlsx
+++ b/src/site/mining.xlsx
@@ -969,11 +969,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3753,8 +3753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5399,7 +5399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="G105" sqref="G105"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5412,11 +5414,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -5489,16 +5491,16 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="E9" s="15" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="E9" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -5694,9 +5696,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
       <c r="E21" s="10" t="s">
         <v>245</v>
       </c>
@@ -5730,27 +5732,27 @@
       </c>
     </row>
     <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:7" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="E27" s="14" t="s">
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="E27" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
     </row>
     <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
@@ -5973,53 +5975,53 @@
       </c>
     </row>
     <row r="39" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="17"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="17"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="16"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="16"/>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="17"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="17"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="16"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="16"/>
     </row>
     <row r="41" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="17"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="16"/>
     </row>
     <row r="42" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="17"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="17"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="16"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="17"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="16"/>
     </row>
     <row r="44" spans="1:7" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="E44" s="14" t="s">
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="E44" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
@@ -6737,16 +6739,16 @@
     <row r="82" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="86" spans="1:7" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A86" s="14" t="s">
+      <c r="A86" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="B86" s="14"/>
-      <c r="C86" s="14"/>
-      <c r="E86" s="14" t="s">
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="E86" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="17"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
@@ -6782,10 +6784,10 @@
         <v>202</v>
       </c>
       <c r="F88" s="10">
-        <v>31217</v>
+        <v>13224</v>
       </c>
       <c r="G88" s="11">
-        <v>236063218390</v>
+        <v>100000000000</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -6998,9 +7000,9 @@
       <c r="C99" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="E99" s="16"/>
-      <c r="F99" s="16"/>
-      <c r="G99" s="16"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="15"/>
+      <c r="G99" s="15"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="10">
@@ -7012,9 +7014,9 @@
       <c r="C100" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="E100" s="16"/>
-      <c r="F100" s="16"/>
-      <c r="G100" s="16"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="15"/>
+      <c r="G100" s="15"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
@@ -7055,10 +7057,10 @@
         <v>202</v>
       </c>
       <c r="F103" s="10">
-        <v>31217</v>
+        <v>13224</v>
       </c>
       <c r="G103" s="11">
-        <v>236063218390</v>
+        <v>100000000000</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -7347,40 +7349,40 @@
       </c>
     </row>
     <row r="126" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="16"/>
-      <c r="B126" s="16"/>
-      <c r="C126" s="17"/>
+      <c r="A126" s="15"/>
+      <c r="B126" s="15"/>
+      <c r="C126" s="16"/>
       <c r="E126"/>
       <c r="F126"/>
       <c r="G126"/>
     </row>
     <row r="127" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="16"/>
-      <c r="B127" s="16"/>
-      <c r="C127" s="17"/>
+      <c r="A127" s="15"/>
+      <c r="B127" s="15"/>
+      <c r="C127" s="16"/>
       <c r="E127"/>
       <c r="F127"/>
       <c r="G127"/>
     </row>
     <row r="128" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="16"/>
-      <c r="B128" s="16"/>
-      <c r="C128" s="17"/>
+      <c r="A128" s="15"/>
+      <c r="B128" s="15"/>
+      <c r="C128" s="16"/>
     </row>
     <row r="129" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="16"/>
-      <c r="B129" s="16"/>
-      <c r="C129" s="17"/>
+      <c r="A129" s="15"/>
+      <c r="B129" s="15"/>
+      <c r="C129" s="16"/>
     </row>
     <row r="130" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="16"/>
-      <c r="B130" s="16"/>
-      <c r="C130" s="17"/>
+      <c r="A130" s="15"/>
+      <c r="B130" s="15"/>
+      <c r="C130" s="16"/>
     </row>
     <row r="131" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="16"/>
-      <c r="B131" s="16"/>
-      <c r="C131" s="17"/>
+      <c r="A131" s="15"/>
+      <c r="B131" s="15"/>
+      <c r="C131" s="16"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E132" s="4"/>
@@ -7394,14 +7396,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E27:G27"/>
     <mergeCell ref="E44:G44"/>
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="E86:G86"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E27:G27"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
verifyTotalParams TestCase and ExecutionType enum
</commit_message>
<xml_diff>
--- a/src/site/mining.xlsx
+++ b/src/site/mining.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="9555" windowHeight="7755"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="9555" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados" sheetId="9" r:id="rId1"/>
@@ -1577,16 +1577,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1884,7 +1912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O203"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2089,7 +2117,7 @@
       <c r="B9" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>2003480</v>
       </c>
       <c r="D9" s="14"/>
@@ -7210,11 +7238,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -7287,11 +7315,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
       <c r="E9" s="13" t="s">
         <v>220</v>
       </c>
@@ -7539,16 +7567,16 @@
     </row>
     <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:7" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="E27" s="17" t="s">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="E27" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -7808,16 +7836,16 @@
       <c r="C43" s="15"/>
     </row>
     <row r="44" spans="1:7" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="E44" s="17" t="s">
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="E44" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
@@ -8535,16 +8563,16 @@
     <row r="82" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="86" spans="1:7" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A86" s="17" t="s">
+      <c r="A86" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="B86" s="17"/>
-      <c r="C86" s="17"/>
-      <c r="E86" s="17" t="s">
+      <c r="B86" s="18"/>
+      <c r="C86" s="18"/>
+      <c r="E86" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="F86" s="17"/>
-      <c r="G86" s="17"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="18"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
@@ -9213,8 +9241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105:B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>